<commit_message>
Demoed code, updated csv files
</commit_message>
<xml_diff>
--- a/results/one_hundred_stats.xlsx
+++ b/results/one_hundred_stats.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="one_hundred" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,8 +1662,8 @@
         <v>1</v>
       </c>
       <c r="B102">
-        <f>MIN(B1:B100)</f>
-        <v>101</v>
+        <f>MAX(B1:B100)</f>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>